<commit_message>
Call amount is now sum of remittance call amounts
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_calls_no_remittances.xlsx
+++ b/public/sample_uploads/capital_calls_no_remittances.xlsx
@@ -1,31 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CD49FB-0A87-48AD-BF17-2DF0AB109ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE57C030-5483-499B-9E65-5495C0FB29BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalCall" sheetId="1" r:id="rId1"/>
+    <sheet name="Exchange Rates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>Fund *</t>
   </si>
@@ -79,6 +75,27 @@
   </si>
   <si>
     <t>CoInvest</t>
+  </si>
+  <si>
+    <t>From Currency</t>
+  </si>
+  <si>
+    <t>To Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange Rate </t>
+  </si>
+  <si>
+    <t>As Of</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -118,8 +135,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +454,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -492,11 +509,11 @@
       <c r="D2">
         <v>30</v>
       </c>
-      <c r="E2" s="1">
-        <v>44905</v>
+      <c r="E2" s="2">
+        <v>44571</v>
       </c>
       <c r="F2" s="2">
-        <v>44914</v>
+        <v>44571</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -521,11 +538,11 @@
       <c r="D3">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
-        <v>44905</v>
+      <c r="E3" s="2">
+        <v>44722</v>
       </c>
       <c r="F3" s="2">
-        <v>44914</v>
+        <v>44722</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -550,11 +567,11 @@
       <c r="D4">
         <v>30</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>44905</v>
       </c>
       <c r="F4" s="2">
-        <v>44914</v>
+        <v>44905</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -570,4 +587,117 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65ED987-63EC-4547-954A-BA0B0A3C517D}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1">
+        <v>81</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>81</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1">
+        <v>82</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>